<commit_message>
Fixed some pathing issue. Made new gerber ffiles. Started making list of parts.
</commit_message>
<xml_diff>
--- a/voice coil BOM.xlsx
+++ b/voice coil BOM.xlsx
@@ -18,12 +18,94 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Example URL</t>
+  </si>
+  <si>
+    <t>3.2uF surface mount capacitors 0805</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/ceramic-multilayer-capacitors/6911161/</t>
+  </si>
+  <si>
+    <t>10k surface mount resistors 0805</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/6789667/</t>
+  </si>
+  <si>
+    <t>5k surface mount resistors 0805</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/6791569/</t>
+  </si>
+  <si>
+    <t>LM324G opamps</t>
+  </si>
+  <si>
+    <t>FMMT449 (NPN transistors)</t>
+  </si>
+  <si>
+    <t>FSB749 (PNP transistors)</t>
+  </si>
+  <si>
+    <t>DAC (AD5338RBRUZ)</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/operational-amplifiers/0858405/</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/bipolar-transistors/6697681/</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/bipolar-transistors/8076033/?searchTerm=FSB749&amp;relevancy-data=636F3D3226696E3D4931384E4B6E6F776E41734D504E266C753D7A68266D6D3D6D61746368616C6C7061727469616C26706D3D5E5B5C772D5C2E2F252C5D2B2426706F3D313326736E3D592673743D4B4559574F52445F53494E474C455F414C5048415F4E554D455249432677633D424F5448267573743D465342373439267374613D46534237343926</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/general-purpose-dacs/8209173/?searchTerm=AD5338RBRUZ&amp;relevancy-data=636F3D3226696E3D4931384E4B6E6F776E41734D504E266C753D7A68266D6D3D6D61746368616C6C7061727469616C26706D3D5E5B5C772D5C2E2F252C5D2B2426706F3D313326736E3D592673743D4B4559574F52445F53494E474C455F414C5048415F4E554D455249432677633D424F5448267573743D414435333338524252555A267374613D414435333338524252555A26</t>
+  </si>
+  <si>
+    <t>1k surface mount resistors 0805</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/8145889/</t>
+  </si>
+  <si>
+    <t>30k surface mount resistors 0805</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/6792039/</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -46,13 +128,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -144,6 +234,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -179,6 +286,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -331,12 +455,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="97" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="B6" r:id="rId4"/>
+    <hyperlink ref="B7" r:id="rId5"/>
+    <hyperlink ref="B8" r:id="rId6" display="http://china.rs-online.com/web/p/bipolar-transistors/8076033/?searchTerm=FSB749&amp;relevancy-data=636F3D3226696E3D4931384E4B6E6F776E41734D504E266C753D7A68266D6D3D6D61746368616C6C7061727469616C26706D3D5E5B5C772D5C2E2F252C5D2B2426706F3D313326736E3D592673743D4B4559574F52445F53494E474C455F414C5048415F4E554D455249432677633D424F5448267573743D465342373439267374613D46534237343926"/>
+    <hyperlink ref="B9" r:id="rId7" display="http://china.rs-online.com/web/p/general-purpose-dacs/8209173/?searchTerm=AD5338RBRUZ&amp;relevancy-data=636F3D3226696E3D4931384E4B6E6F776E41734D504E266C753D7A68266D6D3D6D61746368616C6C7061727469616C26706D3D5E5B5C772D5C2E2F252C5D2B2426706F3D313326736E3D592673743D4B4559574F52445F53494E474C455F414C5048415F4E554D455249432677633D424F5448267573743D414435333338524252555A267374613D414435333338524252555A26"/>
+    <hyperlink ref="B10" r:id="rId8"/>
+    <hyperlink ref="B11" r:id="rId9"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Labels for voice coil components
</commit_message>
<xml_diff>
--- a/voice coil BOM.xlsx
+++ b/voice coil BOM.xlsx
@@ -1,16 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Description</t>
   </si>
@@ -45,9 +48,6 @@
     <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/6791569/</t>
   </si>
   <si>
-    <t>LM324G opamps</t>
-  </si>
-  <si>
     <t>FMMT449 (NPN transistors)</t>
   </si>
   <si>
@@ -81,13 +81,43 @@
     <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/6792039/</t>
   </si>
   <si>
-    <t>Number</t>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>C1, C2, C3, C4</t>
+  </si>
+  <si>
+    <t>R6, R11, R12</t>
+  </si>
+  <si>
+    <t>LM324D opamps</t>
+  </si>
+  <si>
+    <t>U9, U10</t>
+  </si>
+  <si>
+    <t>U3, U4, U7, U8</t>
+  </si>
+  <si>
+    <t>U1, U2, U5, U6</t>
+  </si>
+  <si>
+    <t>DAC1</t>
+  </si>
+  <si>
+    <t>R13, R14</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R4, R7, R8, R9, R10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -201,7 +231,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -253,7 +283,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -447,7 +477,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -458,17 +488,17 @@
   <dimension ref="A2:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
     <col min="2" max="2" width="97" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" customWidth="1"/>
+    <col min="3" max="3" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -476,79 +506,106 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="23">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="23">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="23">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="56">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="56">
+      <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="23">
+      <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="23">
+      <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>19</v>
+      <c r="C11" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -564,6 +621,10 @@
     <hyperlink ref="B11" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated COM and zipped things
</commit_message>
<xml_diff>
--- a/voice coil BOM.xlsx
+++ b/voice coil BOM.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="0" windowWidth="22260" windowHeight="12640"/>
+    <workbookView xWindow="375" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -144,12 +144,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -165,7 +171,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -173,6 +179,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -480,7 +490,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -491,31 +501,31 @@
   <dimension ref="A2:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
     <col min="2" max="2" width="97" customWidth="1"/>
-    <col min="3" max="3" width="34.83203125" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="23">
+    <row r="3" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -529,7 +539,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="23">
+    <row r="4" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -543,7 +553,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="23">
+    <row r="5" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -557,7 +567,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -571,7 +581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -585,7 +595,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="56">
+    <row r="8" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -599,7 +609,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="56">
+    <row r="9" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -613,7 +623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="23">
+    <row r="10" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -627,7 +637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="23">
+    <row r="11" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
corrected BOM, zipped up
</commit_message>
<xml_diff>
--- a/voice coil BOM.xlsx
+++ b/voice coil BOM.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Description</t>
   </si>
@@ -39,9 +39,6 @@
     <t>10k surface mount resistors 0805</t>
   </si>
   <si>
-    <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/6789667/</t>
-  </si>
-  <si>
     <t>5k surface mount resistors 0805</t>
   </si>
   <si>
@@ -72,21 +69,12 @@
     <t>1k surface mount resistors 0805</t>
   </si>
   <si>
-    <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/8145889/</t>
-  </si>
-  <si>
     <t>30k surface mount resistors 0805</t>
   </si>
   <si>
-    <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/6792039/</t>
-  </si>
-  <si>
     <t>Label</t>
   </si>
   <si>
-    <t>C1, C2, C3, C4</t>
-  </si>
-  <si>
     <t>R6, R11, R12</t>
   </si>
   <si>
@@ -115,6 +103,27 @@
   </si>
   <si>
     <t>Quantity</t>
+  </si>
+  <si>
+    <t>C1, C2, C3, C4, C11</t>
+  </si>
+  <si>
+    <t>10 pin female header</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/pcb-sockets/7655745/</t>
+  </si>
+  <si>
+    <t>J1, J2</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/2230427/</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/2230562/</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/6791263/</t>
   </si>
 </sst>
 </file>
@@ -244,7 +253,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -296,7 +305,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -498,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D11"/>
+  <dimension ref="A2:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,10 +528,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
@@ -533,7 +542,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -544,10 +553,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -555,13 +564,13 @@
     </row>
     <row r="5" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D5">
         <v>8</v>
@@ -569,13 +578,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -583,13 +592,13 @@
     </row>
     <row r="7" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D7">
         <v>4</v>
@@ -597,13 +606,13 @@
     </row>
     <row r="8" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D8">
         <v>4</v>
@@ -611,13 +620,13 @@
     </row>
     <row r="9" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -625,13 +634,13 @@
     </row>
     <row r="10" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -639,29 +648,41 @@
     </row>
     <row r="11" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
-    <hyperlink ref="B6" r:id="rId4"/>
-    <hyperlink ref="B7" r:id="rId5"/>
-    <hyperlink ref="B8" r:id="rId6" display="http://china.rs-online.com/web/p/bipolar-transistors/8076033/?searchTerm=FSB749&amp;relevancy-data=636F3D3226696E3D4931384E4B6E6F776E41734D504E266C753D7A68266D6D3D6D61746368616C6C7061727469616C26706D3D5E5B5C772D5C2E2F252C5D2B2426706F3D313326736E3D592673743D4B4559574F52445F53494E474C455F414C5048415F4E554D455249432677633D424F5448267573743D465342373439267374613D46534237343926"/>
-    <hyperlink ref="B9" r:id="rId7" display="http://china.rs-online.com/web/p/general-purpose-dacs/8209173/?searchTerm=AD5338RBRUZ&amp;relevancy-data=636F3D3226696E3D4931384E4B6E6F776E41734D504E266C753D7A68266D6D3D6D61746368616C6C7061727469616C26706D3D5E5B5C772D5C2E2F252C5D2B2426706F3D313326736E3D592673743D4B4559574F52445F53494E474C455F414C5048415F4E554D455249432677633D424F5448267573743D414435333338524252555A267374613D414435333338524252555A26"/>
-    <hyperlink ref="B10" r:id="rId8"/>
-    <hyperlink ref="B11" r:id="rId9"/>
+    <hyperlink ref="B5" r:id="rId2"/>
+    <hyperlink ref="B6" r:id="rId3"/>
+    <hyperlink ref="B7" r:id="rId4"/>
+    <hyperlink ref="B8" r:id="rId5" display="http://china.rs-online.com/web/p/bipolar-transistors/8076033/?searchTerm=FSB749&amp;relevancy-data=636F3D3226696E3D4931384E4B6E6F776E41734D504E266C753D7A68266D6D3D6D61746368616C6C7061727469616C26706D3D5E5B5C772D5C2E2F252C5D2B2426706F3D313326736E3D592673743D4B4559574F52445F53494E474C455F414C5048415F4E554D455249432677633D424F5448267573743D465342373439267374613D46534237343926"/>
+    <hyperlink ref="B9" r:id="rId6" display="http://china.rs-online.com/web/p/general-purpose-dacs/8209173/?searchTerm=AD5338RBRUZ&amp;relevancy-data=636F3D3226696E3D4931384E4B6E6F776E41734D504E266C753D7A68266D6D3D6D61746368616C6C7061727469616C26706D3D5E5B5C772D5C2E2F252C5D2B2426706F3D313326736E3D592673743D4B4559574F52445F53494E474C455F414C5048415F4E554D455249432677633D424F5448267573743D414435333338524252555A267374613D414435333338524252555A26"/>
+    <hyperlink ref="B10" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>